<commit_message>
edit naming and removed auto-population table shells
</commit_message>
<xml_diff>
--- a/4.01 Protocol for Preparing Datasets/Example Variables for Feed the Future ZOI Survey Datasets_20220405.xlsx
+++ b/4.01 Protocol for Preparing Datasets/Example Variables for Feed the Future ZOI Survey Datasets_20220405.xlsx
@@ -27794,8 +27794,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011A3E5F9AA6593439116F79CA10376F1" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aa81e6f34497b5dee97a50b007a245c4">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d58e8a2-dff7-4492-a987-8cd66a35f019" xmlns:ns3="a7a5a0b0-47c5-4056-9505-4cb74804ae11" xmlns:ns4="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ce02d3080834df40a3c73274b843bea0" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011A3E5F9AA6593439116F79CA10376F1" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="45fa2a71bb5685042c59d1fbaafccb6b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d58e8a2-dff7-4492-a987-8cd66a35f019" xmlns:ns3="a7a5a0b0-47c5-4056-9505-4cb74804ae11" xmlns:ns4="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3afdd82834536de8985540a519edf7e7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="0d58e8a2-dff7-4492-a987-8cd66a35f019"/>
     <xsd:import namespace="a7a5a0b0-47c5-4056-9505-4cb74804ae11"/>
     <xsd:import namespace="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe"/>
@@ -27819,6 +27819,7 @@
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns2:DLVStatus" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -27894,6 +27895,11 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -28063,7 +28069,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0833BDFB-C00A-4156-8674-738CB7A7F102}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B25A2471-61EE-4ECF-9EC8-CECAA47926BD}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>